<commit_message>
Adding standards sheet to example input
</commit_message>
<xml_diff>
--- a/data/input/20190822 - GHG - Lauren - SD and Dief samples.xlsx
+++ b/data/input/20190822 - GHG - Lauren - SD and Dief samples.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinwhitfield/Documents/work_vm/Research/UoS/Bigfoot/GC_v2-1_code/Raw Data/GCtest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\GC_v3\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAA79053-7A00-844B-9545-B24AD0E10876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1100" windowWidth="25040" windowHeight="13800"/>
+    <workbookView xWindow="480" yWindow="1100" windowWidth="25040" windowHeight="13800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="20190822 - GHG - Lauren - SD an" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="244">
   <si>
     <t>file</t>
   </si>
@@ -749,12 +749,15 @@
   </si>
   <si>
     <t>C:\CompassCDS\Data\2019\08\22\08_22_2019 19_11_29_R6_V1_lab air.DATA</t>
+  </si>
+  <si>
+    <t>STANDARD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1232,9 +1235,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1592,11 +1598,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="39.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +1699,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1780,7 +1791,7 @@
         <v>0.30191273099999999</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1872,7 +1883,7 @@
         <v>0.301745873</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1964,7 +1975,7 @@
         <v>0.100000063</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -2056,7 +2067,7 @@
         <v>0.29314675699999998</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2148,7 +2159,7 @@
         <v>0.69600299899999996</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2240,7 +2251,7 @@
         <v>0.98900540199999998</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>11.842334640000001</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2424,7 +2435,7 @@
         <v>625.35835210000005</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -2516,7 +2527,7 @@
         <v>0.32656869999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2608,7 +2619,7 @@
         <v>0.100979294</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -2700,7 +2711,7 @@
         <v>0.29665602600000002</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -2792,7 +2803,7 @@
         <v>0.305158928</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -2884,7 +2895,7 @@
         <v>0.30360387999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>54</v>
       </c>
@@ -2976,7 +2987,7 @@
         <v>0.26948881899999999</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -3068,7 +3079,7 @@
         <v>0.273166403</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -3160,7 +3171,7 @@
         <v>0.29621956199999999</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -3252,7 +3263,7 @@
         <v>0.26363174900000003</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3344,7 +3355,7 @@
         <v>0.293499913</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -3436,7 +3447,7 @@
         <v>0.34428440599999999</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -3528,7 +3539,7 @@
         <v>0.36556704600000001</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -3620,7 +3631,7 @@
         <v>1.151288208</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>70</v>
       </c>
@@ -3712,7 +3723,7 @@
         <v>0.98852321899999995</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -3804,7 +3815,7 @@
         <v>0.29379608800000001</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -3896,7 +3907,7 @@
         <v>0.29518949100000003</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>76</v>
       </c>
@@ -3988,7 +3999,7 @@
         <v>0.29745077199999997</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -4080,7 +4091,7 @@
         <v>0.29856223799999998</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>80</v>
       </c>
@@ -4172,7 +4183,7 @@
         <v>0.29672422900000001</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -4264,7 +4275,7 @@
         <v>0.299071115</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -4356,7 +4367,7 @@
         <v>0.29879538500000002</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -4448,7 +4459,7 @@
         <v>0.29884820200000001</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -4540,7 +4551,7 @@
         <v>0.30313655299999998</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -4632,7 +4643,7 @@
         <v>0.34348460200000003</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -4724,7 +4735,7 @@
         <v>0.34702497799999998</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>94</v>
       </c>
@@ -4816,7 +4827,7 @@
         <v>0.29487165399999998</v>
       </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -4908,7 +4919,7 @@
         <v>0.29922035299999999</v>
       </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -5000,7 +5011,7 @@
         <v>0.28302034500000001</v>
       </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -5092,7 +5103,7 @@
         <v>0.28640161200000003</v>
       </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -5184,7 +5195,7 @@
         <v>0.37115271900000002</v>
       </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>104</v>
       </c>
@@ -5276,7 +5287,7 @@
         <v>0.35553500700000001</v>
       </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -5368,7 +5379,7 @@
         <v>0.29211564699999998</v>
       </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -5460,7 +5471,7 @@
         <v>0.28896430499999998</v>
       </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -5552,7 +5563,7 @@
         <v>0.303780249</v>
       </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>112</v>
       </c>
@@ -5644,7 +5655,7 @@
         <v>0.30372070400000001</v>
       </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -5736,7 +5747,7 @@
         <v>0.25877008299999998</v>
       </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>116</v>
       </c>
@@ -5828,7 +5839,7 @@
         <v>0.25983864899999998</v>
       </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>118</v>
       </c>
@@ -5920,7 +5931,7 @@
         <v>0.30034993599999998</v>
       </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>120</v>
       </c>
@@ -6012,7 +6023,7 @@
         <v>0.27672825600000001</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>122</v>
       </c>
@@ -6104,7 +6115,7 @@
         <v>0.28452818699999999</v>
       </c>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>124</v>
       </c>
@@ -6196,7 +6207,7 @@
         <v>0.30301739999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>126</v>
       </c>
@@ -6288,7 +6299,7 @@
         <v>0.27625736499999998</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>128</v>
       </c>
@@ -6380,7 +6391,7 @@
         <v>0.27840127399999998</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>130</v>
       </c>
@@ -6472,7 +6483,7 @@
         <v>0.30772576099999999</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>132</v>
       </c>
@@ -6564,7 +6575,7 @@
         <v>0.28108956400000001</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>134</v>
       </c>
@@ -6656,7 +6667,7 @@
         <v>0.28027630199999998</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>136</v>
       </c>
@@ -6748,7 +6759,7 @@
         <v>8.1616157999999994E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -6840,7 +6851,7 @@
         <v>8.9460599000000002E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -6932,7 +6943,7 @@
         <v>0.22562015899999999</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>142</v>
       </c>
@@ -7024,7 +7035,7 @@
         <v>0.22379095299999999</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>144</v>
       </c>
@@ -7116,7 +7127,7 @@
         <v>0.26857594899999998</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>146</v>
       </c>
@@ -7208,7 +7219,7 @@
         <v>0.25770726700000002</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>148</v>
       </c>
@@ -7300,7 +7311,7 @@
         <v>0.25438722699999999</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>150</v>
       </c>
@@ -7392,7 +7403,7 @@
         <v>0.25284402499999997</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>152</v>
       </c>
@@ -7484,7 +7495,7 @@
         <v>1.0254066879999999</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>154</v>
       </c>
@@ -7576,7 +7587,7 @@
         <v>0.30288304199999999</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>155</v>
       </c>
@@ -7668,7 +7679,7 @@
         <v>0.100192456</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>156</v>
       </c>
@@ -7760,7 +7771,7 @@
         <v>0.29271204200000001</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>157</v>
       </c>
@@ -7852,7 +7863,7 @@
         <v>0.30399488000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>158</v>
       </c>
@@ -7944,7 +7955,7 @@
         <v>1.0767496999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>160</v>
       </c>
@@ -8036,7 +8047,7 @@
         <v>2.1591667819999998</v>
       </c>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>162</v>
       </c>
@@ -8128,7 +8139,7 @@
         <v>2.1683517069999998</v>
       </c>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>164</v>
       </c>
@@ -8220,7 +8231,7 @@
         <v>0.179337724</v>
       </c>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>166</v>
       </c>
@@ -8312,7 +8323,7 @@
         <v>0.1756363</v>
       </c>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>168</v>
       </c>
@@ -8404,7 +8415,7 @@
         <v>0.20335514900000001</v>
       </c>
     </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>170</v>
       </c>
@@ -8496,7 +8507,7 @@
         <v>0.214113837</v>
       </c>
     </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>172</v>
       </c>
@@ -8588,7 +8599,7 @@
         <v>0.23366131500000001</v>
       </c>
     </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -8680,7 +8691,7 @@
         <v>0.23367068999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>176</v>
       </c>
@@ -8772,7 +8783,7 @@
         <v>0.27488467300000002</v>
       </c>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>178</v>
       </c>
@@ -8864,7 +8875,7 @@
         <v>0.272898802</v>
       </c>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>180</v>
       </c>
@@ -8956,7 +8967,7 @@
         <v>0.230337233</v>
       </c>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>182</v>
       </c>
@@ -9048,7 +9059,7 @@
         <v>0.22730292899999999</v>
       </c>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>184</v>
       </c>
@@ -9140,7 +9151,7 @@
         <v>0.24954781600000001</v>
       </c>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>186</v>
       </c>
@@ -9232,7 +9243,7 @@
         <v>0.25519792600000002</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>188</v>
       </c>
@@ -9324,7 +9335,7 @@
         <v>0.120928681</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>190</v>
       </c>
@@ -9416,7 +9427,7 @@
         <v>0.123750558</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>192</v>
       </c>
@@ -9508,7 +9519,7 @@
         <v>0.24944993300000001</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>194</v>
       </c>
@@ -9600,7 +9611,7 @@
         <v>0.25030898099999999</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>196</v>
       </c>
@@ -9692,7 +9703,7 @@
         <v>0.276422004</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>198</v>
       </c>
@@ -9784,7 +9795,7 @@
         <v>0.27699012200000001</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>200</v>
       </c>
@@ -9876,7 +9887,7 @@
         <v>0.280539492</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>202</v>
       </c>
@@ -9968,7 +9979,7 @@
         <v>0.287393597</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>204</v>
       </c>
@@ -10060,7 +10071,7 @@
         <v>0.225654248</v>
       </c>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>206</v>
       </c>
@@ -10152,7 +10163,7 @@
         <v>0.22740065700000001</v>
       </c>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>208</v>
       </c>
@@ -10244,7 +10255,7 @@
         <v>0.193873352</v>
       </c>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>210</v>
       </c>
@@ -10336,7 +10347,7 @@
         <v>0.18972583500000001</v>
       </c>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>212</v>
       </c>
@@ -10428,7 +10439,7 @@
         <v>8.7859977000000006E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>214</v>
       </c>
@@ -10520,7 +10531,7 @@
         <v>8.4999587000000001E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>216</v>
       </c>
@@ -10612,7 +10623,7 @@
         <v>0.209423</v>
       </c>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>218</v>
       </c>
@@ -10704,7 +10715,7 @@
         <v>0.20458304599999999</v>
       </c>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>220</v>
       </c>
@@ -10796,7 +10807,7 @@
         <v>0.28019429699999998</v>
       </c>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>222</v>
       </c>
@@ -10888,7 +10899,7 @@
         <v>0.26205012599999999</v>
       </c>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>224</v>
       </c>
@@ -10980,7 +10991,7 @@
         <v>0.28608403700000001</v>
       </c>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>226</v>
       </c>
@@ -11072,7 +11083,7 @@
         <v>0.27568035899999999</v>
       </c>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>228</v>
       </c>
@@ -11164,7 +11175,7 @@
         <v>0.306386349</v>
       </c>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>230</v>
       </c>
@@ -11256,7 +11267,7 @@
         <v>0.30273951300000002</v>
       </c>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>232</v>
       </c>
@@ -11348,7 +11359,7 @@
         <v>0.29944995200000002</v>
       </c>
     </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>233</v>
       </c>
@@ -11440,7 +11451,7 @@
         <v>0.30141764900000001</v>
       </c>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>234</v>
       </c>
@@ -11532,7 +11543,7 @@
         <v>0.10984071099999999</v>
       </c>
     </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>235</v>
       </c>
@@ -11624,7 +11635,7 @@
         <v>0.29366708600000002</v>
       </c>
     </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>236</v>
       </c>
@@ -11716,7 +11727,7 @@
         <v>0.69689789000000002</v>
       </c>
     </row>
-    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>237</v>
       </c>
@@ -11808,7 +11819,7 @@
         <v>0.98671017500000002</v>
       </c>
     </row>
-    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>238</v>
       </c>
@@ -11900,7 +11911,7 @@
         <v>11.79429712</v>
       </c>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>239</v>
       </c>
@@ -11992,7 +12003,7 @@
         <v>623.52502030000005</v>
       </c>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>240</v>
       </c>
@@ -12084,7 +12095,7 @@
         <v>0.32210930100000001</v>
       </c>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>241</v>
       </c>
@@ -12176,7 +12187,7 @@
         <v>0.30841505499999999</v>
       </c>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>242</v>
       </c>
@@ -12271,4 +12282,86 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.08203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>0.31709999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>0.69599999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>9.52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>